<commit_message>
Issue#17  REQ 3.1  implement logic for reading sample excel file  GREEN TEST for creating SAP models from SAMPLE XLSX file  there's potential bug in excel file where last row can be empty but in  reality will cause nullpointer exception  you can achieve this by insert new row after last one with data
</commit_message>
<xml_diff>
--- a/Sample_SAP_DevMan_20180821.xlsx
+++ b/Sample_SAP_DevMan_20180821.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitLab\hr-tools\devman-generator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Library\devman-generator-v2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,14 +15,14 @@
     <sheet name="Samples" sheetId="4" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Samples!$A$1:$K$28</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Samples!$A$1:$K$27</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="145">
   <si>
     <t>First name</t>
   </si>
@@ -54,15 +54,9 @@
     <t>Rybczyńska</t>
   </si>
   <si>
-    <t>AARK</t>
-  </si>
-  <si>
     <t>Staff</t>
   </si>
   <si>
-    <t>Rybczyńska Anna</t>
-  </si>
-  <si>
     <t>Corporate Services</t>
   </si>
   <si>
@@ -198,9 +192,6 @@
     <t>600272</t>
   </si>
   <si>
-    <t>Jakub</t>
-  </si>
-  <si>
     <t>600126</t>
   </si>
   <si>
@@ -403,9 +394,6 @@
   </si>
   <si>
     <t>Banasiak</t>
-  </si>
-  <si>
-    <t>Nowogórski</t>
   </si>
   <si>
     <t>Legal</t>
@@ -1304,10 +1292,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K28"/>
+  <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="A27" sqref="A27:XFD27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1337,7 +1325,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -1355,322 +1343,322 @@
         <v>7</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="E2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>13</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>15</v>
       </c>
       <c r="I2" s="5">
         <v>41764</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I3" s="5">
         <v>39295</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="I4" s="5">
         <v>39342</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="I5" s="5">
         <v>39342</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I6" s="5">
         <v>39388</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I7" s="5">
         <v>39433</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="I8" s="5"/>
       <c r="J8" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="I9" s="5"/>
       <c r="J9" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="I10" s="5"/>
       <c r="J10" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="I11" s="5"/>
       <c r="J11" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="I12" s="5"/>
       <c r="J12" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
@@ -1678,300 +1666,297 @@
         <v>8</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="I13" s="5"/>
       <c r="J13" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="I14" s="5"/>
       <c r="J14" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="I15" s="5"/>
       <c r="J15" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="I16" s="5"/>
       <c r="J16" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="K16" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="I17" s="5"/>
       <c r="J17" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="K17" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="I18" s="5"/>
       <c r="J18" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="K18" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="I19" s="5"/>
       <c r="J19" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="K19" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="I20" s="5"/>
       <c r="J20" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="K20" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="I21" s="5"/>
       <c r="J21" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="K21" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="I22" s="5"/>
       <c r="J22" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="K22" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="I23" s="5"/>
       <c r="J23" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="K23" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="I24" s="5"/>
       <c r="J24" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="K24" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="I25" s="5"/>
       <c r="J25" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="K25" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="I26" s="5"/>
       <c r="J26" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="K26" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="I27" s="5"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="I28" s="5"/>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:K28"/>
+  <autoFilter ref="A1:K27"/>
   <sortState ref="F3:F11">
     <sortCondition ref="F2"/>
   </sortState>

</xml_diff>

<commit_message>
Issue#17  REQ 3.1  GREEN UNIT TEST  a lot of refactor to lambdas, streams
Issue#17
 REQ 3.1
 BUG if in excel somebody inserted empty row

EOD

all phases of refactor

Issue#17
 REQ 3.1
 GREEN UNIT TEST
 a lot of refactor to lambdas, streams
</commit_message>
<xml_diff>
--- a/Sample_SAP_DevMan_20180821.xlsx
+++ b/Sample_SAP_DevMan_20180821.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Samples" sheetId="4" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Samples!$A$1:$K$27</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Samples!$A$1:$K$28</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
@@ -1292,7 +1292,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K27"/>
+  <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A27" sqref="A27:XFD27"/>
@@ -1955,8 +1955,11 @@
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="I27" s="5"/>
     </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I28" s="5"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:K27"/>
+  <autoFilter ref="A1:K28"/>
   <sortState ref="F3:F11">
     <sortCondition ref="F2"/>
   </sortState>

</xml_diff>

<commit_message>
Issue#17  REQ 3.1  ADD GREEN UNIT TEST for scenario in which SAP generates additional column   refactor
</commit_message>
<xml_diff>
--- a/Sample_SAP_DevMan_20180821.xlsx
+++ b/Sample_SAP_DevMan_20180821.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="146">
   <si>
     <t>First name</t>
   </si>
@@ -457,6 +457,9 @@
   </si>
   <si>
     <t>e-SRSK</t>
+  </si>
+  <si>
+    <t>dupa</t>
   </si>
 </sst>
 </file>
@@ -1292,10 +1295,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K28"/>
+  <dimension ref="A1:L28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27:XFD27"/>
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1314,7 +1317,7 @@
     <col min="12" max="16384" width="11.42578125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="3" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" s="3" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1348,8 +1351,11 @@
       <c r="K1" s="1" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L1" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>73</v>
       </c>
@@ -1383,8 +1389,11 @@
       <c r="K2" s="4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L2" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>79</v>
       </c>
@@ -1418,8 +1427,11 @@
       <c r="K3" s="4" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L3" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>48</v>
       </c>
@@ -1447,8 +1459,11 @@
       <c r="K4" s="4" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L4" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>87</v>
       </c>
@@ -1476,8 +1491,11 @@
       <c r="K5" s="4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L5" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>58</v>
       </c>
@@ -1505,8 +1523,11 @@
       <c r="K6" s="4" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L6" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>90</v>
       </c>
@@ -1534,8 +1555,11 @@
       <c r="K7" s="4" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L7" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>121</v>
       </c>
@@ -1561,8 +1585,11 @@
       <c r="K8" s="4" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L8" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>102</v>
       </c>
@@ -1588,8 +1615,11 @@
       <c r="K9" s="4" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L9" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>114</v>
       </c>
@@ -1615,8 +1645,11 @@
       <c r="K10" s="4" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L10" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>75</v>
       </c>
@@ -1639,8 +1672,11 @@
       <c r="K11" s="4" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L11" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>107</v>
       </c>
@@ -1660,8 +1696,11 @@
       <c r="K12" s="4" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L12" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>8</v>
       </c>
@@ -1681,8 +1720,11 @@
       <c r="K13" s="4" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L13" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>71</v>
       </c>
@@ -1702,8 +1744,11 @@
       <c r="K14" s="4" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L14" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>76</v>
       </c>
@@ -1723,8 +1768,11 @@
       <c r="K15" s="4" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L15" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>72</v>
       </c>
@@ -1744,8 +1792,11 @@
       <c r="K16" s="4" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L16" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>60</v>
       </c>
@@ -1765,8 +1816,11 @@
       <c r="K17" s="4" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L17" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>63</v>
       </c>
@@ -1786,8 +1840,11 @@
       <c r="K18" s="4" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L18" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>42</v>
       </c>
@@ -1807,8 +1864,11 @@
       <c r="K19" s="4" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L19" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>113</v>
       </c>
@@ -1828,8 +1888,11 @@
       <c r="K20" s="4" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L20" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>104</v>
       </c>
@@ -1849,8 +1912,11 @@
       <c r="K21" s="4" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L21" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>129</v>
       </c>
@@ -1870,8 +1936,11 @@
       <c r="K22" s="4" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L22" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
         <v>94</v>
       </c>
@@ -1891,8 +1960,11 @@
       <c r="K23" s="4" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L23" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>29</v>
       </c>
@@ -1912,8 +1984,11 @@
       <c r="K24" s="4" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L24" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
         <v>95</v>
       </c>
@@ -1933,8 +2008,11 @@
       <c r="K25" s="4" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L25" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>80</v>
       </c>
@@ -1951,11 +2029,14 @@
       <c r="K26" s="4" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L26" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="I27" s="5"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="I28" s="5"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Issue#17   RED UNIT TEST IOEXCEPTION
</commit_message>
<xml_diff>
--- a/Sample_SAP_DevMan_20180821.xlsx
+++ b/Sample_SAP_DevMan_20180821.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="145">
   <si>
     <t>First name</t>
   </si>
@@ -457,9 +457,6 @@
   </si>
   <si>
     <t>e-SRSK</t>
-  </si>
-  <si>
-    <t>dupa</t>
   </si>
 </sst>
 </file>
@@ -1295,10 +1292,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L28"/>
+  <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+      <selection activeCell="L1" sqref="L1:L1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1317,7 +1314,7 @@
     <col min="12" max="16384" width="11.42578125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="3" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" s="3" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1351,11 +1348,8 @@
       <c r="K1" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="L1" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>73</v>
       </c>
@@ -1389,11 +1383,8 @@
       <c r="K2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="L2" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>79</v>
       </c>
@@ -1427,11 +1418,8 @@
       <c r="K3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="L3" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>48</v>
       </c>
@@ -1459,11 +1447,8 @@
       <c r="K4" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="L4" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>87</v>
       </c>
@@ -1491,11 +1476,8 @@
       <c r="K5" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="L5" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>58</v>
       </c>
@@ -1523,11 +1505,8 @@
       <c r="K6" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="L6" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>90</v>
       </c>
@@ -1555,11 +1534,8 @@
       <c r="K7" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="L7" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>121</v>
       </c>
@@ -1585,11 +1561,8 @@
       <c r="K8" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="L8" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>102</v>
       </c>
@@ -1615,11 +1588,8 @@
       <c r="K9" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="L9" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>114</v>
       </c>
@@ -1645,11 +1615,8 @@
       <c r="K10" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="L10" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>75</v>
       </c>
@@ -1672,11 +1639,8 @@
       <c r="K11" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="L11" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>107</v>
       </c>
@@ -1696,11 +1660,8 @@
       <c r="K12" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="L12" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>8</v>
       </c>
@@ -1720,11 +1681,8 @@
       <c r="K13" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="L13" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>71</v>
       </c>
@@ -1744,11 +1702,8 @@
       <c r="K14" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="L14" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>76</v>
       </c>
@@ -1768,11 +1723,8 @@
       <c r="K15" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="L15" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>72</v>
       </c>
@@ -1792,11 +1744,8 @@
       <c r="K16" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="L16" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>60</v>
       </c>
@@ -1816,11 +1765,8 @@
       <c r="K17" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="L17" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>63</v>
       </c>
@@ -1840,11 +1786,8 @@
       <c r="K18" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="L18" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>42</v>
       </c>
@@ -1864,11 +1807,8 @@
       <c r="K19" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="L19" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>113</v>
       </c>
@@ -1888,11 +1828,8 @@
       <c r="K20" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="L20" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>104</v>
       </c>
@@ -1912,11 +1849,8 @@
       <c r="K21" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="L21" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>129</v>
       </c>
@@ -1936,11 +1870,8 @@
       <c r="K22" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="L22" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
         <v>94</v>
       </c>
@@ -1960,11 +1891,8 @@
       <c r="K23" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="L23" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>29</v>
       </c>
@@ -1984,11 +1912,8 @@
       <c r="K24" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="L24" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
         <v>95</v>
       </c>
@@ -2008,11 +1933,8 @@
       <c r="K25" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="L25" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>80</v>
       </c>
@@ -2029,14 +1951,11 @@
       <c r="K26" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="L26" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="I27" s="5"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="I28" s="5"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Issue#17  REQ 3.1   refactor notNullRows method to stream
</commit_message>
<xml_diff>
--- a/Sample_SAP_DevMan_20180821.xlsx
+++ b/Sample_SAP_DevMan_20180821.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Samples" sheetId="4" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Samples!$A$1:$K$28</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Samples!$A$1:$K$26</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
@@ -1292,10 +1292,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K28"/>
+  <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:L1048576"/>
+      <selection activeCell="A27" sqref="A27:XFD27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1955,11 +1955,8 @@
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="I27" s="5"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="I28" s="5"/>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:K28"/>
+  <autoFilter ref="A1:K26"/>
   <sortState ref="F3:F11">
     <sortCondition ref="F2"/>
   </sortState>

</xml_diff>

<commit_message>
fixing pull from master
</commit_message>
<xml_diff>
--- a/Sample_SAP_DevMan_20180821.xlsx
+++ b/Sample_SAP_DevMan_20180821.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitLab\hr-tools\devman-generator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Library\devman-generator-v2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,14 +15,14 @@
     <sheet name="Samples" sheetId="4" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Samples!$A$1:$K$28</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Samples!$A$1:$K$26</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="145">
   <si>
     <t>First name</t>
   </si>
@@ -54,15 +54,9 @@
     <t>Rybczyńska</t>
   </si>
   <si>
-    <t>AARK</t>
-  </si>
-  <si>
     <t>Staff</t>
   </si>
   <si>
-    <t>Rybczyńska Anna</t>
-  </si>
-  <si>
     <t>Corporate Services</t>
   </si>
   <si>
@@ -198,9 +192,6 @@
     <t>600272</t>
   </si>
   <si>
-    <t>Jakub</t>
-  </si>
-  <si>
     <t>600126</t>
   </si>
   <si>
@@ -403,9 +394,6 @@
   </si>
   <si>
     <t>Banasiak</t>
-  </si>
-  <si>
-    <t>Nowogórski</t>
   </si>
   <si>
     <t>Legal</t>
@@ -1304,10 +1292,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K28"/>
+  <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="A27" sqref="A27:XFD27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1337,7 +1325,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -1355,322 +1343,322 @@
         <v>7</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="E2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>13</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>15</v>
       </c>
       <c r="I2" s="5">
         <v>41764</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I3" s="5">
         <v>39295</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="I4" s="5">
         <v>39342</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="I5" s="5">
         <v>39342</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I6" s="5">
         <v>39388</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I7" s="5">
         <v>39433</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="I8" s="5"/>
       <c r="J8" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="I9" s="5"/>
       <c r="J9" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="I10" s="5"/>
       <c r="J10" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="I11" s="5"/>
       <c r="J11" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="I12" s="5"/>
       <c r="J12" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
@@ -1678,300 +1666,297 @@
         <v>8</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="I13" s="5"/>
       <c r="J13" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="I14" s="5"/>
       <c r="J14" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="I15" s="5"/>
       <c r="J15" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="I16" s="5"/>
       <c r="J16" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="K16" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="I17" s="5"/>
       <c r="J17" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="K17" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="I18" s="5"/>
       <c r="J18" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="K18" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="I19" s="5"/>
       <c r="J19" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="K19" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="I20" s="5"/>
       <c r="J20" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="K20" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="I21" s="5"/>
       <c r="J21" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="K21" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="I22" s="5"/>
       <c r="J22" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="K22" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="I23" s="5"/>
       <c r="J23" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="K23" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="I24" s="5"/>
       <c r="J24" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="K24" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="I25" s="5"/>
       <c r="J25" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="K25" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="I26" s="5"/>
       <c r="J26" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="K26" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="I27" s="5"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="I28" s="5"/>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:K28"/>
+  <autoFilter ref="A1:K26"/>
   <sortState ref="F3:F11">
     <sortCondition ref="F2"/>
   </sortState>

</xml_diff>

<commit_message>
Issue#23 Req 3.3  changes to template files on remote repository
</commit_message>
<xml_diff>
--- a/Sample_SAP_DevMan_20180821.xlsx
+++ b/Sample_SAP_DevMan_20180821.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Library\devman-generator-v2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Library\devman-generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -36,9 +36,6 @@
     <t>Employee Subgroup</t>
   </si>
   <si>
-    <t>Position</t>
-  </si>
-  <si>
     <t>Job</t>
   </si>
   <si>
@@ -457,6 +454,9 @@
   </si>
   <si>
     <t>e-SRSK</t>
+  </si>
+  <si>
+    <t>Job Family</t>
   </si>
 </sst>
 </file>
@@ -1295,7 +1295,7 @@
   <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27:XFD27"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1325,631 +1325,631 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="J1" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>12</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>13</v>
       </c>
       <c r="I2" s="5">
         <v>41764</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I3" s="5">
         <v>39295</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I4" s="5">
         <v>39342</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I5" s="5">
         <v>39342</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I6" s="5">
         <v>39388</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I7" s="5">
         <v>39433</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I8" s="5"/>
       <c r="J8" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I9" s="5"/>
       <c r="J9" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I10" s="5"/>
       <c r="J10" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I11" s="5"/>
       <c r="J11" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I12" s="5"/>
       <c r="J12" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I13" s="5"/>
       <c r="J13" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I14" s="5"/>
       <c r="J14" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I15" s="5"/>
       <c r="J15" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I16" s="5"/>
       <c r="J16" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K16" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I17" s="5"/>
       <c r="J17" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K17" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I18" s="5"/>
       <c r="J18" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K18" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I19" s="5"/>
       <c r="J19" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K19" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="I20" s="5"/>
       <c r="J20" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K20" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I21" s="5"/>
       <c r="J21" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K21" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I22" s="5"/>
       <c r="J22" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K22" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I23" s="5"/>
       <c r="J23" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K23" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I24" s="5"/>
       <c r="J24" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K24" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I25" s="5"/>
       <c r="J25" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K25" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I26" s="5"/>
       <c r="J26" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K26" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Issue#23 Req 3.3  SAP init entry column is used to calculate seniority please check SAPMentoringModel javadocs
</commit_message>
<xml_diff>
--- a/Sample_SAP_DevMan_20180821.xlsx
+++ b/Sample_SAP_DevMan_20180821.xlsx
@@ -15,14 +15,14 @@
     <sheet name="Samples" sheetId="4" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Samples!$A$1:$K$26</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Samples!$B$1:$K$26</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="146">
   <si>
     <t>First name</t>
   </si>
@@ -457,6 +457,9 @@
   </si>
   <si>
     <t>Job Family</t>
+  </si>
+  <si>
+    <t>Date of Birth</t>
   </si>
 </sst>
 </file>
@@ -602,7 +605,7 @@
       <charset val="238"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -780,6 +783,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDDDDD"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -958,7 +967,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -969,6 +978,10 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -1292,20 +1305,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K27"/>
+  <dimension ref="A1:L27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.5703125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" style="4" customWidth="1"/>
-    <col min="6" max="6" width="22.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5703125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" style="4" customWidth="1"/>
     <col min="7" max="7" width="15" style="4" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="21" style="4" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.7109375" style="4" bestFit="1" customWidth="1"/>
@@ -1314,24 +1327,24 @@
     <col min="12" max="16384" width="11.42578125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="3" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" s="3" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>144</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>4</v>
@@ -1348,25 +1361,28 @@
       <c r="K1" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L1" s="6" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="C2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>9</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>10</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>11</v>
@@ -1383,25 +1399,28 @@
       <c r="K2" s="4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L2" s="7">
+        <v>33442</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="C3" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="E3" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="F3" s="4" t="s">
         <v>43</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>29</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>132</v>
@@ -1419,18 +1438,18 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="C4" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="E4" s="4" t="s">
         <v>77</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>52</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>99</v>
@@ -1448,18 +1467,18 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="C5" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="E5" s="4" t="s">
         <v>36</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>88</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>63</v>
@@ -1477,18 +1496,18 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="C6" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="E6" s="4" t="s">
         <v>50</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>49</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>30</v>
@@ -1506,18 +1525,18 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="C7" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="E7" s="4" t="s">
         <v>82</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>38</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>15</v>
@@ -1535,18 +1554,18 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="C8" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="E8" s="4" t="s">
         <v>107</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>20</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>18</v>
@@ -1562,18 +1581,18 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="C9" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="E9" s="4" t="s">
         <v>65</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>25</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>35</v>
@@ -1589,18 +1608,18 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="C10" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="E10" s="4" t="s">
         <v>55</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>14</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>21</v>
@@ -1616,18 +1635,18 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="C11" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="E11" s="4" t="s">
         <v>64</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>33</v>
       </c>
       <c r="H11" s="4" t="s">
         <v>76</v>
@@ -1640,14 +1659,14 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B12" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="C12" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="E12" s="4" t="s">
         <v>67</v>
       </c>
       <c r="H12" s="4" t="s">
@@ -1661,14 +1680,14 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B13" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="C13" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="E13" s="4" t="s">
         <v>61</v>
       </c>
       <c r="H13" s="4" t="s">
@@ -1682,14 +1701,14 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B14" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="C14" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="E14" s="4" t="s">
         <v>140</v>
       </c>
       <c r="H14" s="4" t="s">
@@ -1703,14 +1722,14 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B15" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="C15" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="E15" s="4" t="s">
         <v>141</v>
       </c>
       <c r="H15" s="4" t="s">
@@ -1724,14 +1743,14 @@
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A16" s="4" t="s">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B16" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="C16" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="E16" s="4" t="s">
         <v>142</v>
       </c>
       <c r="H16" s="4" t="s">
@@ -1745,14 +1764,14 @@
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A17" s="4" t="s">
+    <row r="17" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B17" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="C17" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="E17" s="4" t="s">
         <v>84</v>
       </c>
       <c r="H17" s="4" t="s">
@@ -1766,14 +1785,14 @@
         <v>48</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B18" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="C18" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="E18" s="4" t="s">
         <v>32</v>
       </c>
       <c r="H18" s="4" t="s">
@@ -1787,14 +1806,14 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A19" s="4" t="s">
+    <row r="19" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B19" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="C19" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="E19" s="4" t="s">
         <v>51</v>
       </c>
       <c r="H19" s="4" t="s">
@@ -1808,14 +1827,14 @@
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A20" s="4" t="s">
+    <row r="20" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B20" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="C20" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="E20" s="4" t="s">
         <v>19</v>
       </c>
       <c r="H20" s="4" t="s">
@@ -1829,14 +1848,14 @@
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A21" s="4" t="s">
+    <row r="21" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B21" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="C21" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="E21" s="4" t="s">
         <v>81</v>
       </c>
       <c r="H21" s="4" t="s">
@@ -1850,14 +1869,14 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A22" s="4" t="s">
+    <row r="22" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B22" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="C22" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="E22" s="4" t="s">
         <v>102</v>
       </c>
       <c r="H22" s="4" t="s">
@@ -1871,14 +1890,14 @@
         <v>51</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A23" s="4" t="s">
+    <row r="23" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B23" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="C23" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="E23" s="4" t="s">
         <v>48</v>
       </c>
       <c r="H23" s="4" t="s">
@@ -1892,14 +1911,14 @@
         <v>50</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A24" s="4" t="s">
+    <row r="24" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B24" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="C24" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="D24" s="4" t="s">
+      <c r="E24" s="4" t="s">
         <v>124</v>
       </c>
       <c r="H24" s="4" t="s">
@@ -1913,14 +1932,14 @@
         <v>53</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A25" s="4" t="s">
+    <row r="25" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B25" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="C25" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="D25" s="4" t="s">
+      <c r="E25" s="4" t="s">
         <v>69</v>
       </c>
       <c r="H25" s="4" t="s">
@@ -1934,14 +1953,14 @@
         <v>54</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A26" s="4" t="s">
+    <row r="26" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B26" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="C26" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="D26" s="4" t="s">
+      <c r="E26" s="4" t="s">
         <v>73</v>
       </c>
       <c r="I26" s="5"/>
@@ -1952,13 +1971,13 @@
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:11" x14ac:dyDescent="0.2">
       <c r="I27" s="5"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K26"/>
-  <sortState ref="F3:F11">
-    <sortCondition ref="F2"/>
+  <autoFilter ref="B1:K26"/>
+  <sortState ref="A3:A11">
+    <sortCondition ref="A2"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Issue#23 Req 3.3  add date of birth column  try excelvalidator this reads additional column name
</commit_message>
<xml_diff>
--- a/Sample_SAP_DevMan_20180821.xlsx
+++ b/Sample_SAP_DevMan_20180821.xlsx
@@ -1308,7 +1308,7 @@
   <dimension ref="A1:L27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+      <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1437,6 +1437,9 @@
       <c r="K3" s="4" t="s">
         <v>17</v>
       </c>
+      <c r="L3" s="7">
+        <v>33443</v>
+      </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
@@ -1466,6 +1469,9 @@
       <c r="K4" s="4" t="s">
         <v>19</v>
       </c>
+      <c r="L4" s="7">
+        <v>33444</v>
+      </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
@@ -1495,6 +1501,9 @@
       <c r="K5" s="4" t="s">
         <v>23</v>
       </c>
+      <c r="L5" s="7">
+        <v>33445</v>
+      </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
@@ -1524,6 +1533,9 @@
       <c r="K6" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="L6" s="7">
+        <v>33446</v>
+      </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
@@ -1553,6 +1565,9 @@
       <c r="K7" s="4" t="s">
         <v>31</v>
       </c>
+      <c r="L7" s="7">
+        <v>33447</v>
+      </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
@@ -1580,6 +1595,9 @@
       <c r="K8" s="4" t="s">
         <v>32</v>
       </c>
+      <c r="L8" s="7">
+        <v>33448</v>
+      </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
@@ -1607,6 +1625,9 @@
       <c r="K9" s="4" t="s">
         <v>34</v>
       </c>
+      <c r="L9" s="7">
+        <v>33449</v>
+      </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
@@ -1634,6 +1655,9 @@
       <c r="K10" s="4" t="s">
         <v>36</v>
       </c>
+      <c r="L10" s="7">
+        <v>33450</v>
+      </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
@@ -1658,6 +1682,9 @@
       <c r="K11" s="4" t="s">
         <v>36</v>
       </c>
+      <c r="L11" s="7">
+        <v>33451</v>
+      </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B12" s="4" t="s">
@@ -1679,6 +1706,9 @@
       <c r="K12" s="4" t="s">
         <v>39</v>
       </c>
+      <c r="L12" s="7">
+        <v>33452</v>
+      </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B13" s="4" t="s">
@@ -1700,6 +1730,9 @@
       <c r="K13" s="4" t="s">
         <v>40</v>
       </c>
+      <c r="L13" s="7">
+        <v>33453</v>
+      </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B14" s="4" t="s">
@@ -1721,6 +1754,9 @@
       <c r="K14" s="4" t="s">
         <v>42</v>
       </c>
+      <c r="L14" s="7">
+        <v>33454</v>
+      </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B15" s="4" t="s">
@@ -1742,6 +1778,9 @@
       <c r="K15" s="4" t="s">
         <v>45</v>
       </c>
+      <c r="L15" s="7">
+        <v>33455</v>
+      </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B16" s="4" t="s">
@@ -1763,8 +1802,11 @@
       <c r="K16" s="4" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L16" s="7">
+        <v>33456</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B17" s="4" t="s">
         <v>59</v>
       </c>
@@ -1784,8 +1826,11 @@
       <c r="K17" s="4" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L17" s="7">
+        <v>33457</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B18" s="4" t="s">
         <v>62</v>
       </c>
@@ -1805,8 +1850,11 @@
       <c r="K18" s="4" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L18" s="7">
+        <v>33458</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B19" s="4" t="s">
         <v>41</v>
       </c>
@@ -1826,8 +1874,11 @@
       <c r="K19" s="4" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L19" s="7">
+        <v>33459</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B20" s="4" t="s">
         <v>112</v>
       </c>
@@ -1847,8 +1898,11 @@
       <c r="K20" s="4" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L20" s="7">
+        <v>33460</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B21" s="4" t="s">
         <v>103</v>
       </c>
@@ -1868,8 +1922,11 @@
       <c r="K21" s="4" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L21" s="7">
+        <v>33461</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B22" s="4" t="s">
         <v>128</v>
       </c>
@@ -1889,8 +1946,11 @@
       <c r="K22" s="4" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L22" s="7">
+        <v>33462</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B23" s="4" t="s">
         <v>93</v>
       </c>
@@ -1910,8 +1970,11 @@
       <c r="K23" s="4" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L23" s="7">
+        <v>33463</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B24" s="4" t="s">
         <v>28</v>
       </c>
@@ -1931,8 +1994,11 @@
       <c r="K24" s="4" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L24" s="7">
+        <v>33464</v>
+      </c>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B25" s="4" t="s">
         <v>94</v>
       </c>
@@ -1952,8 +2018,11 @@
       <c r="K25" s="4" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L25" s="7">
+        <v>33465</v>
+      </c>
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B26" s="4" t="s">
         <v>79</v>
       </c>
@@ -1970,8 +2039,11 @@
       <c r="K26" s="4" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L26" s="7">
+        <v>33466</v>
+      </c>
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.2">
       <c r="I27" s="5"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Issue#23 Req 3.3  add date of birth column  fix all test from test-class#3 and test-clasa#  fixes were due to difficult data generation
</commit_message>
<xml_diff>
--- a/Sample_SAP_DevMan_20180821.xlsx
+++ b/Sample_SAP_DevMan_20180821.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11700"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11703"/>
   </bookViews>
   <sheets>
     <sheet name="Samples" sheetId="4" r:id="rId1"/>
@@ -1308,26 +1308,26 @@
   <dimension ref="A1:L27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N18" sqref="N18"/>
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.375" defaultRowHeight="12.45" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.5703125" style="4" customWidth="1"/>
-    <col min="6" max="6" width="11.140625" style="4" customWidth="1"/>
+    <col min="1" max="1" width="22.125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.375" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.875" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.625" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="11.125" style="4" customWidth="1"/>
     <col min="7" max="7" width="15" style="4" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="21" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.75" style="4" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13" style="4" customWidth="1"/>
-    <col min="11" max="11" width="10.5703125" style="4" customWidth="1"/>
-    <col min="12" max="16384" width="11.42578125" style="4"/>
+    <col min="11" max="11" width="10.625" style="4" customWidth="1"/>
+    <col min="12" max="16384" width="11.375" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="3" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" s="3" customFormat="1" ht="38.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>144</v>
       </c>
@@ -1626,7 +1626,7 @@
         <v>34</v>
       </c>
       <c r="L9" s="7">
-        <v>33449</v>
+        <v>36737</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Issue#27 Req 3.5  3.5 Add Personnel Subarea column in SAP file  add column requires 11 red tests to be rewritten
</commit_message>
<xml_diff>
--- a/Sample_SAP_DevMan_20180821.xlsx
+++ b/Sample_SAP_DevMan_20180821.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="150">
   <si>
     <t>First name</t>
   </si>
@@ -460,6 +460,18 @@
   </si>
   <si>
     <t>Date of Birth</t>
+  </si>
+  <si>
+    <t>Personnel Subarea</t>
+  </si>
+  <si>
+    <t>Warsaw</t>
+  </si>
+  <si>
+    <t>Lodz</t>
+  </si>
+  <si>
+    <t>Poznan</t>
   </si>
 </sst>
 </file>
@@ -967,7 +979,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -984,6 +996,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1305,10 +1318,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L27"/>
+  <dimension ref="A1:M27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.375" defaultRowHeight="12.45" x14ac:dyDescent="0.2"/>
@@ -1324,10 +1337,12 @@
     <col min="9" max="9" width="10.75" style="4" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13" style="4" customWidth="1"/>
     <col min="11" max="11" width="10.625" style="4" customWidth="1"/>
-    <col min="12" max="16384" width="11.375" style="4"/>
+    <col min="12" max="12" width="11.375" style="4"/>
+    <col min="13" max="13" width="16.625" style="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="11.375" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="3" customFormat="1" ht="38.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" s="3" customFormat="1" ht="38.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>144</v>
       </c>
@@ -1364,8 +1379,11 @@
       <c r="L1" s="6" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M1" s="6" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>10</v>
       </c>
@@ -1402,8 +1420,11 @@
       <c r="L2" s="7">
         <v>33442</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>29</v>
       </c>
@@ -1440,8 +1461,11 @@
       <c r="L3" s="7">
         <v>33443</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M3" s="8" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>52</v>
       </c>
@@ -1472,8 +1496,11 @@
       <c r="L4" s="7">
         <v>33444</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M4" s="8" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>88</v>
       </c>
@@ -1505,7 +1532,7 @@
         <v>33445</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>49</v>
       </c>
@@ -1537,7 +1564,7 @@
         <v>33446</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>38</v>
       </c>
@@ -1569,7 +1596,7 @@
         <v>33447</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>20</v>
       </c>
@@ -1599,7 +1626,7 @@
         <v>33448</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>25</v>
       </c>
@@ -1629,7 +1656,7 @@
         <v>36737</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>14</v>
       </c>
@@ -1659,7 +1686,7 @@
         <v>33450</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>33</v>
       </c>
@@ -1686,7 +1713,7 @@
         <v>33451</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B12" s="4" t="s">
         <v>106</v>
       </c>
@@ -1710,7 +1737,7 @@
         <v>33452</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B13" s="4" t="s">
         <v>7</v>
       </c>
@@ -1734,7 +1761,7 @@
         <v>33453</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B14" s="4" t="s">
         <v>70</v>
       </c>
@@ -1758,7 +1785,7 @@
         <v>33454</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B15" s="4" t="s">
         <v>75</v>
       </c>
@@ -1782,7 +1809,7 @@
         <v>33455</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B16" s="4" t="s">
         <v>71</v>
       </c>

</xml_diff>